<commit_message>
Releaseplan um 1. Sprint-Plan erweitert.
</commit_message>
<xml_diff>
--- a/swe-iot/docs/it000/Releaseplan.xlsx
+++ b/swe-iot/docs/it000/Releaseplan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Scrum-Master:</t>
   </si>
@@ -48,29 +48,35 @@
     <t>Sprint 1:</t>
   </si>
   <si>
-    <t>2. Implementieren Sie die Methoden zum Setzen der Leds und zum Abschalten der Leds. Schreiben Sie auch dafŸr einen Test der ohne den Button aus kommt. Schreiben Sie auch eine kleine Applikation die zeigt, wie die LEDS gesetzt und gelšscht werden (LedDemoApp).</t>
-  </si>
-  <si>
-    <t>3. Implementieren Sie die Methoden zum Abfragen und ZurŸcksetzen der Button ZŠhler. Schreiben Sie auch eine kleine Applikation die ZŠhler ausliest und zurŸcksetzt (ButtonCounterDemo).</t>
-  </si>
-  <si>
-    <t>1. Implementieren Sie die Funktion zum Abspielen eines Tones in der InternetButtonApiImpl. Schreiben Sie auch eine kleine Applikation die zeigt, dass die Melodie auch wirklich ertšnt (PlayDemoApp).</t>
-  </si>
-  <si>
     <t>Stories:</t>
   </si>
   <si>
-    <t>StoryPoints</t>
-  </si>
-  <si>
     <t>Sprint 3:</t>
   </si>
   <si>
     <t>Sprint 2:</t>
   </si>
   <si>
+    <t>Sprint 4:</t>
+  </si>
+  <si>
+    <t>Sprint 5:</t>
+  </si>
+  <si>
+    <t>Sprint 6:</t>
+  </si>
+  <si>
+    <t>Rollenbeschreibung</t>
+  </si>
+  <si>
+    <t>E1S1 Implementieren Sie die Funktion zum Abspielen eines Tones in der InternetButtonApiImpl. Schreiben Sie auch eine kleine Applikation die zeigt, dass die Melodie auch wirklich ertšnt (PlayDemoApp).</t>
+  </si>
+  <si>
+    <t>E1S3 Implementieren Sie die Methoden zum Abfragen und ZurŸcksetzen der Button ZŠhler. Schreiben Sie auch eine kleine Applikation die ZŠhler ausliest und zurŸcksetzt (ButtonCounterDemo).</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">1. Die Klasse </t>
+      <t xml:space="preserve">E2S1 Die Klasse </t>
     </r>
     <r>
       <rPr>
@@ -90,20 +96,17 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1. Erstellen Sie eine neue Klasse und ändern Sie das Verhalten so ab, dass bei jedem Klick die Farbe immer einen stärkeren rot Anteil bekommt (10er Schritte beim Farbwert). Beim Erreichen, des vollen Rot Anteils (255) soll der Zähler zurück gesetzt werden. Zeigen Sie das wieder anhand eines Tests. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Es soll ein neues Verhalten implementiert werden, dass bei allen 10 Klicks eine Melodie abspielt. </t>
-  </si>
-  <si>
-    <t>Sprint 4:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Erweitern Sie die Interfaces so, dass die es einzelne Methoden zur abfrage des x,y, und z wertes des Beschleuniguns Sensors zu Verfügung stehen. Schreiben sie dazu wieder zuerst Testfälle und zeigen Sie die Implementierung in einem kleinen Demo. </t>
+    <t xml:space="preserve">E2S2 Erstellen Sie eine neue Klasse und ändern Sie das Verhalten so ab, dass bei jedem Klick die Farbe immer einen stärkeren rot Anteil bekommt (10er Schritte beim Farbwert). Beim Erreichen, des vollen Rot Anteils (255) soll der Zähler zurück gesetzt werden. Zeigen Sie das wieder anhand eines Tests. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E2S3 Es soll ein neues Verhalten implementiert werden, dass bei allen 10 Klicks eine Melodie abspielt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E3S1 Erweitern Sie die Interfaces so, dass die es einzelne Methoden zur abfrage des x,y, und z wertes des Beschleuniguns Sensors zu Verfügung stehen. Schreiben sie dazu wieder zuerst Testfälle und zeigen Sie die Implementierung in einem kleinen Demo. </t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">2. Erstellen die ein Verhalten ähnlich dem in der Klasse </t>
+      <t xml:space="preserve">E3S2 Erstellen die ein Verhalten ähnlich dem in der Klasse </t>
     </r>
     <r>
       <rPr>
@@ -123,11 +126,14 @@
     </r>
   </si>
   <si>
-    <t>Sprint 5:</t>
+    <t xml:space="preserve">E4S2 Ermöglichen Sie es, dass man eine andere Melodie Spielen kann (Beispiele haben die Lektoren). Dazu muss in der Firmware ein Parameter für die Melodie angegeben werden. Wieder Testfälle und Demo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E4S1 Ermöglichen Sie es, dass mehrerer Leds auf einmal gesetzt werden können. Dazu muss eine neue Methode in der Firmware umgesetzt werden und es sollen die entsprechenden HighLevel API Methode angeboten werden. Wieder Testfälle und Demo. </t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1. Erstellen die ein Verhalten ähnlich dem in der Klasse </t>
+      <t xml:space="preserve">E3S3 Erstellen die ein Verhalten ähnlich dem in der Klasse </t>
     </r>
     <r>
       <rPr>
@@ -147,16 +153,52 @@
     </r>
   </si>
   <si>
-    <t>Sprint 6:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Ermöglichen Sie es, dass mehrerer Leds auf einmal gesetzt werden können. Dazu muss eine neue Methode in der Firmware umgesetzt werden und es sollen die entsprechenden HighLevel API Methode angeboten werden. Wieder Testfälle und Demo. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Ermöglichen Sie es, dass man eine andere Melodie Spielen kann (Beispiele haben die Lektoren). Dazu muss in der Firmware ein Parameter für die Melodie angegeben werden. Wieder Testfälle und Demo. </t>
-  </si>
-  <si>
-    <t>Rollenbeschreibung</t>
+    <t>1. Aufgabe</t>
+  </si>
+  <si>
+    <t>Methode implementieren zum Abspielen des Tons.</t>
+  </si>
+  <si>
+    <t>Wer?</t>
+  </si>
+  <si>
+    <t>2. Aufgabe</t>
+  </si>
+  <si>
+    <t>3. Aufgabe</t>
+  </si>
+  <si>
+    <t>4. Aufgabe</t>
+  </si>
+  <si>
+    <t>E1S2 Implementieren Sie die Methoden zum Setzen der Leds und zum Abschalten der Leds. Schreiben Sie auch dafür einen Test der ohne den Button aus kommt. Schreiben Sie auch eine kleine Applikation die zeigt, wie die LEDS gesetzt und gelšscht werden (LedDemoApp).</t>
+  </si>
+  <si>
+    <t>Methode zum Setzen und Abschalten der LEDs implementieren</t>
+  </si>
+  <si>
+    <t>Test-first-Ansatz: Testmethode zum Ein-/Ausschalten der LEDs schreiben</t>
+  </si>
+  <si>
+    <t>Aufrufer implementieren</t>
+  </si>
+  <si>
+    <t>LedDemoApp Leds aus- und einschalten. (SOS)</t>
+  </si>
+  <si>
+    <t>5. Aufgabe</t>
+  </si>
+  <si>
+    <t>Christian, Philipp</t>
+  </si>
+  <si>
+    <t>Georg, Stefan</t>
+  </si>
+  <si>
+    <t>Michael, Markus</t>
+  </si>
+  <si>
+    <t>Storypoints</t>
   </si>
 </sst>
 </file>
@@ -240,7 +282,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -253,36 +295,49 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="14">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -612,202 +667,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:18" ht="23">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:18">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:18">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:18">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:18">
       <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:18">
       <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:18">
       <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:18">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+    </row>
+    <row r="13" spans="1:18" ht="91" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:18" ht="100" customHeight="1">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="74" customHeight="1">
+      <c r="E15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="7">
+        <v>3</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7">
+        <v>3</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7">
+        <v>3</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7">
+        <v>2</v>
+      </c>
+      <c r="O15" s="7"/>
+      <c r="P15">
         <v>12</v>
       </c>
-      <c r="F12" s="3" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="17" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="98" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" ht="148" customHeight="1">
+      <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="98" customHeight="1">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" ht="93" customHeight="1">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="100" customHeight="1">
+      <c r="A26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" ht="80" customHeight="1">
+      <c r="A28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="66" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="100" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="74" customHeight="1"/>
-    <row r="17" spans="1:3" ht="17" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="98" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" ht="148" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="5" t="s">
+    <row r="31" spans="1:3" ht="86" customHeight="1">
+      <c r="A31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" ht="86" customHeight="1">
+      <c r="A32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="98" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" ht="93" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="100" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" ht="80" customHeight="1">
-      <c r="A28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="86" customHeight="1">
-      <c r="A31" s="2" t="s">
+    <row r="35" spans="1:3" ht="85" customHeight="1">
+      <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" ht="86" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="4"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="85" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Doku.txt gelöscht (war nur für die Ordnererstellung notwendig) Releaseplan aktualisiert SprintPlan erstellt
</commit_message>
<xml_diff>
--- a/swe-iot/docs/it000/Releaseplan.xlsx
+++ b/swe-iot/docs/it000/Releaseplan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15683" windowHeight="2618" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Scrum-Master:</t>
   </si>
@@ -153,52 +154,7 @@
     </r>
   </si>
   <si>
-    <t>1. Aufgabe</t>
-  </si>
-  <si>
-    <t>Methode implementieren zum Abspielen des Tons.</t>
-  </si>
-  <si>
-    <t>Wer?</t>
-  </si>
-  <si>
-    <t>2. Aufgabe</t>
-  </si>
-  <si>
-    <t>3. Aufgabe</t>
-  </si>
-  <si>
-    <t>4. Aufgabe</t>
-  </si>
-  <si>
     <t>E1S2 Implementieren Sie die Methoden zum Setzen der Leds und zum Abschalten der Leds. Schreiben Sie auch dafür einen Test der ohne den Button aus kommt. Schreiben Sie auch eine kleine Applikation die zeigt, wie die LEDS gesetzt und gelšscht werden (LedDemoApp).</t>
-  </si>
-  <si>
-    <t>Methode zum Setzen und Abschalten der LEDs implementieren</t>
-  </si>
-  <si>
-    <t>Test-first-Ansatz: Testmethode zum Ein-/Ausschalten der LEDs schreiben</t>
-  </si>
-  <si>
-    <t>Aufrufer implementieren</t>
-  </si>
-  <si>
-    <t>LedDemoApp Leds aus- und einschalten. (SOS)</t>
-  </si>
-  <si>
-    <t>5. Aufgabe</t>
-  </si>
-  <si>
-    <t>Christian, Philipp</t>
-  </si>
-  <si>
-    <t>Georg, Stefan</t>
-  </si>
-  <si>
-    <t>Michael, Markus</t>
-  </si>
-  <si>
-    <t>Storypoints</t>
   </si>
 </sst>
 </file>
@@ -208,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -306,12 +262,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -323,25 +273,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -669,18 +633,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="17.8125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.8125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="23">
+    <row r="1" spans="1:18" ht="23.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -735,123 +699,67 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" ht="91.05" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="100.05" customHeight="1">
+      <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="1:18" ht="91" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="1:18" ht="100" customHeight="1">
-      <c r="A14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
     </row>
     <row r="15" spans="1:18" ht="74" customHeight="1">
-      <c r="E15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="7">
-        <v>3</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7">
-        <v>1</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7">
-        <v>3</v>
-      </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7">
-        <v>3</v>
-      </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7">
-        <v>2</v>
-      </c>
-      <c r="O15" s="7"/>
-      <c r="P15">
-        <v>12</v>
-      </c>
+      <c r="E15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="17" spans="1:3" ht="17" customHeight="1">
       <c r="A17" s="2" t="s">
@@ -859,18 +767,18 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="98" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" ht="148" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" ht="148.05000000000001" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
@@ -878,42 +786,42 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="98" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" ht="93" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="100" customHeight="1">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:3" ht="100.05" customHeight="1">
+      <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:3" ht="80" customHeight="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
@@ -921,18 +829,18 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="86" customHeight="1">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" ht="86" customHeight="1">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1"/>
@@ -942,27 +850,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="85" customHeight="1">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:3" ht="85.05" customHeight="1">
+      <c r="A35" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>